<commit_message>
test commit with clined repo
</commit_message>
<xml_diff>
--- a/02_grocery_app/02_02_prepared_data/recipebook.xlsx
+++ b/02_grocery_app/02_02_prepared_data/recipebook.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25427"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25601"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lewis\venv\python310\python-masterclass-remaster-shared\finances\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lewis\venv\python310\python-masterclass-remaster-shared\personal_projects\02_grocery_app\02_02_prepared_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C3FAAE11-D894-4411-AD92-15B9863030F8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A0FBFFB9-F95B-4734-8023-E927ADEC7B1D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{1B25F3A4-3DC7-4B1C-B390-8500E0CADD3E}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="461" uniqueCount="107">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1025" uniqueCount="170">
   <si>
     <t>Recipe Title</t>
   </si>
@@ -356,6 +356,195 @@
   </si>
   <si>
     <t>fruit</t>
+  </si>
+  <si>
+    <t>Meal</t>
+  </si>
+  <si>
+    <t>dinner</t>
+  </si>
+  <si>
+    <t>dessert</t>
+  </si>
+  <si>
+    <t>Tomato Egg noodle soup</t>
+  </si>
+  <si>
+    <t xml:space="preserve">tomatoes </t>
+  </si>
+  <si>
+    <t>chinese noodles</t>
+  </si>
+  <si>
+    <t>chicken broth</t>
+  </si>
+  <si>
+    <t>cilantro</t>
+  </si>
+  <si>
+    <t>lunch</t>
+  </si>
+  <si>
+    <t>Shakshuka</t>
+  </si>
+  <si>
+    <t>olive oil</t>
+  </si>
+  <si>
+    <t>red bell pepper</t>
+  </si>
+  <si>
+    <t>paprika</t>
+  </si>
+  <si>
+    <t>cumin</t>
+  </si>
+  <si>
+    <t>can</t>
+  </si>
+  <si>
+    <t>parsley</t>
+  </si>
+  <si>
+    <t>breakfast</t>
+  </si>
+  <si>
+    <t>Sammys Lunch</t>
+  </si>
+  <si>
+    <t>cauliflour</t>
+  </si>
+  <si>
+    <t>chicken breast</t>
+  </si>
+  <si>
+    <t>lettuce</t>
+  </si>
+  <si>
+    <t>head</t>
+  </si>
+  <si>
+    <t>lemon</t>
+  </si>
+  <si>
+    <t>white vinegar</t>
+  </si>
+  <si>
+    <t>Steamed Egg *MWL</t>
+  </si>
+  <si>
+    <t>https://seonkyounglongest.com/taiwanese-beef-noodle-soup/print/32100/</t>
+  </si>
+  <si>
+    <t>Taiwanese Beef Noodle Soup</t>
+  </si>
+  <si>
+    <t>cardamom</t>
+  </si>
+  <si>
+    <t>star anise</t>
+  </si>
+  <si>
+    <t>licorice</t>
+  </si>
+  <si>
+    <t>sichuan peppercorn</t>
+  </si>
+  <si>
+    <t>fennel</t>
+  </si>
+  <si>
+    <t>goji berry</t>
+  </si>
+  <si>
+    <t>beef shank</t>
+  </si>
+  <si>
+    <t>shaoxing wine</t>
+  </si>
+  <si>
+    <t>dark soy sauce</t>
+  </si>
+  <si>
+    <t>beef bouillon</t>
+  </si>
+  <si>
+    <t>dry wheat noodles</t>
+  </si>
+  <si>
+    <t>per serving</t>
+  </si>
+  <si>
+    <t>https://www.recipetineats.com/wprm_print/36115</t>
+  </si>
+  <si>
+    <t>Pho</t>
+  </si>
+  <si>
+    <t>coriander</t>
+  </si>
+  <si>
+    <t>beef brisket</t>
+  </si>
+  <si>
+    <t>meaty beef bones</t>
+  </si>
+  <si>
+    <t>marrow bones</t>
+  </si>
+  <si>
+    <t>fish sauce</t>
+  </si>
+  <si>
+    <t>beef tenderloin</t>
+  </si>
+  <si>
+    <t>beansprout</t>
+  </si>
+  <si>
+    <t>basil</t>
+  </si>
+  <si>
+    <t>lime</t>
+  </si>
+  <si>
+    <t>hoisin sauce</t>
+  </si>
+  <si>
+    <t>sriracha</t>
+  </si>
+  <si>
+    <t>spice</t>
+  </si>
+  <si>
+    <t>https://www.bbcgoodfood.com/recipes/ultimate-spaghetti-carbonara-recipe</t>
+  </si>
+  <si>
+    <t>pancetta</t>
+  </si>
+  <si>
+    <t>pecorino cheese</t>
+  </si>
+  <si>
+    <t>parmesan</t>
+  </si>
+  <si>
+    <t>spaghetti</t>
+  </si>
+  <si>
+    <t>Carbonara pasta</t>
+  </si>
+  <si>
+    <t>pea</t>
+  </si>
+  <si>
+    <t>corn</t>
+  </si>
+  <si>
+    <t>https://www.madewithlau.com/recipes/egg-drop-soup</t>
+  </si>
+  <si>
+    <t>Egg drop soup/corn soup *MWL</t>
   </si>
 </sst>
 </file>
@@ -399,10 +588,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -717,21 +907,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4BDFF1AD-754D-44A3-ABE3-C9196CBC2C47}">
-  <dimension ref="A1:E115"/>
+  <dimension ref="A1:G204"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A100" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="E116" sqref="E116"/>
+    <sheetView tabSelected="1" topLeftCell="A119" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="J130" sqref="J130"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="22.7265625" customWidth="1"/>
+    <col min="1" max="1" width="25" customWidth="1"/>
     <col min="2" max="2" width="21.26953125" customWidth="1"/>
     <col min="4" max="4" width="15.90625" customWidth="1"/>
-    <col min="5" max="5" width="14.90625" customWidth="1"/>
+    <col min="5" max="5" width="20.54296875" customWidth="1"/>
+    <col min="6" max="6" width="16.453125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -747,8 +938,11 @@
       <c r="E1" s="2" t="s">
         <v>99</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F1" s="2" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -764,8 +958,11 @@
       <c r="E2" t="s">
         <v>100</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F2" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -781,8 +978,11 @@
       <c r="E3" t="s">
         <v>101</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F3" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>1</v>
       </c>
@@ -799,8 +999,11 @@
       <c r="E4" t="s">
         <v>101</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F4" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>1</v>
       </c>
@@ -816,8 +1019,11 @@
       <c r="E5" t="s">
         <v>101</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F5" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>1</v>
       </c>
@@ -833,8 +1039,11 @@
       <c r="E6" t="s">
         <v>102</v>
       </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F6" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>1</v>
       </c>
@@ -850,8 +1059,11 @@
       <c r="E7" t="s">
         <v>103</v>
       </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F7" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>1</v>
       </c>
@@ -867,8 +1079,11 @@
       <c r="E8" t="s">
         <v>101</v>
       </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F8" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>1</v>
       </c>
@@ -884,8 +1099,11 @@
       <c r="E9" t="s">
         <v>102</v>
       </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F9" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>1</v>
       </c>
@@ -901,8 +1119,11 @@
       <c r="E10" t="s">
         <v>101</v>
       </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F10" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>1</v>
       </c>
@@ -918,8 +1139,11 @@
       <c r="E11" t="s">
         <v>102</v>
       </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F11" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>17</v>
       </c>
@@ -935,8 +1159,11 @@
       <c r="E12" t="s">
         <v>101</v>
       </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F12" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>17</v>
       </c>
@@ -952,8 +1179,11 @@
       <c r="E13" t="s">
         <v>104</v>
       </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F13" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>17</v>
       </c>
@@ -969,8 +1199,11 @@
       <c r="E14" t="s">
         <v>104</v>
       </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F14" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>17</v>
       </c>
@@ -986,8 +1219,11 @@
       <c r="E15" t="s">
         <v>104</v>
       </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F15" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>17</v>
       </c>
@@ -1003,8 +1239,11 @@
       <c r="E16" t="s">
         <v>101</v>
       </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F16" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>17</v>
       </c>
@@ -1020,8 +1259,11 @@
       <c r="E17" t="s">
         <v>102</v>
       </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F17" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>17</v>
       </c>
@@ -1037,8 +1279,11 @@
       <c r="E18" t="s">
         <v>101</v>
       </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F18" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>17</v>
       </c>
@@ -1054,8 +1299,11 @@
       <c r="E19" t="s">
         <v>104</v>
       </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F19" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>17</v>
       </c>
@@ -1071,8 +1319,11 @@
       <c r="E20" t="s">
         <v>104</v>
       </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F20" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>17</v>
       </c>
@@ -1088,8 +1339,11 @@
       <c r="E21" t="s">
         <v>105</v>
       </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F21" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>17</v>
       </c>
@@ -1105,8 +1359,11 @@
       <c r="E22" t="s">
         <v>104</v>
       </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F22" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>17</v>
       </c>
@@ -1122,8 +1379,11 @@
       <c r="E23" t="s">
         <v>104</v>
       </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F23" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
         <v>27</v>
       </c>
@@ -1139,8 +1399,11 @@
       <c r="E24" t="s">
         <v>103</v>
       </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F24" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
         <v>27</v>
       </c>
@@ -1156,8 +1419,11 @@
       <c r="E25" t="s">
         <v>101</v>
       </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F25" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
         <v>27</v>
       </c>
@@ -1173,8 +1439,11 @@
       <c r="E26" t="s">
         <v>101</v>
       </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F26" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
         <v>27</v>
       </c>
@@ -1190,8 +1459,11 @@
       <c r="E27" t="s">
         <v>101</v>
       </c>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F27" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
         <v>27</v>
       </c>
@@ -1207,8 +1479,11 @@
       <c r="E28" t="s">
         <v>103</v>
       </c>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F28" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
         <v>27</v>
       </c>
@@ -1224,8 +1499,11 @@
       <c r="E29" t="s">
         <v>103</v>
       </c>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F29" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
         <v>27</v>
       </c>
@@ -1241,8 +1519,11 @@
       <c r="E30" t="s">
         <v>101</v>
       </c>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F30" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
         <v>27</v>
       </c>
@@ -1258,8 +1539,11 @@
       <c r="E31" t="s">
         <v>101</v>
       </c>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F31" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
         <v>36</v>
       </c>
@@ -1275,8 +1559,11 @@
       <c r="E32" t="s">
         <v>101</v>
       </c>
-    </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F32" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
         <v>36</v>
       </c>
@@ -1292,8 +1579,11 @@
       <c r="E33" t="s">
         <v>101</v>
       </c>
-    </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F33" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
         <v>36</v>
       </c>
@@ -1309,8 +1599,11 @@
       <c r="E34" t="s">
         <v>103</v>
       </c>
-    </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F34" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
         <v>36</v>
       </c>
@@ -1326,8 +1619,11 @@
       <c r="E35" t="s">
         <v>101</v>
       </c>
-    </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F35" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
         <v>36</v>
       </c>
@@ -1343,8 +1639,11 @@
       <c r="E36" t="s">
         <v>101</v>
       </c>
-    </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F36" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
         <v>36</v>
       </c>
@@ -1360,8 +1659,11 @@
       <c r="E37" t="s">
         <v>103</v>
       </c>
-    </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F37" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
         <v>36</v>
       </c>
@@ -1377,8 +1679,11 @@
       <c r="E38" t="s">
         <v>101</v>
       </c>
-    </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F38" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A39" t="s">
         <v>36</v>
       </c>
@@ -1394,8 +1699,11 @@
       <c r="E39" t="s">
         <v>101</v>
       </c>
-    </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F39" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A40" t="s">
         <v>36</v>
       </c>
@@ -1411,8 +1719,11 @@
       <c r="E40" t="s">
         <v>106</v>
       </c>
-    </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F40" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A41" t="s">
         <v>36</v>
       </c>
@@ -1428,8 +1739,11 @@
       <c r="E41" t="s">
         <v>101</v>
       </c>
-    </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F41" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A42" t="s">
         <v>36</v>
       </c>
@@ -1445,8 +1759,11 @@
       <c r="E42" t="s">
         <v>101</v>
       </c>
-    </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F42" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A43" t="s">
         <v>36</v>
       </c>
@@ -1462,8 +1779,11 @@
       <c r="E43" t="s">
         <v>101</v>
       </c>
-    </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F43" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A44" t="s">
         <v>65</v>
       </c>
@@ -1479,8 +1799,11 @@
       <c r="E44" t="s">
         <v>100</v>
       </c>
-    </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F44" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A45" t="s">
         <v>65</v>
       </c>
@@ -1496,8 +1819,11 @@
       <c r="E45" t="s">
         <v>105</v>
       </c>
-    </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F45" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A46" t="s">
         <v>65</v>
       </c>
@@ -1513,8 +1839,11 @@
       <c r="E46" t="s">
         <v>105</v>
       </c>
-    </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F46" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A47" t="s">
         <v>65</v>
       </c>
@@ -1530,8 +1859,11 @@
       <c r="E47" t="s">
         <v>102</v>
       </c>
-    </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F47" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A48" t="s">
         <v>65</v>
       </c>
@@ -1547,8 +1879,11 @@
       <c r="E48" t="s">
         <v>101</v>
       </c>
-    </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F48" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A49" t="s">
         <v>65</v>
       </c>
@@ -1564,8 +1899,11 @@
       <c r="E49" t="s">
         <v>102</v>
       </c>
-    </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F49" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A50" t="s">
         <v>45</v>
       </c>
@@ -1581,8 +1919,11 @@
       <c r="E50" t="s">
         <v>100</v>
       </c>
-    </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F50" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A51" t="s">
         <v>45</v>
       </c>
@@ -1598,8 +1939,11 @@
       <c r="E51" t="s">
         <v>101</v>
       </c>
-    </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F51" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A52" t="s">
         <v>45</v>
       </c>
@@ -1615,8 +1959,11 @@
       <c r="E52" t="s">
         <v>101</v>
       </c>
-    </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F52" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A53" t="s">
         <v>45</v>
       </c>
@@ -1632,8 +1979,11 @@
       <c r="E53" t="s">
         <v>102</v>
       </c>
-    </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F53" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A54" t="s">
         <v>45</v>
       </c>
@@ -1649,8 +1999,11 @@
       <c r="E54" t="s">
         <v>105</v>
       </c>
-    </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F54" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A55" t="s">
         <v>45</v>
       </c>
@@ -1666,8 +2019,11 @@
       <c r="E55" t="s">
         <v>105</v>
       </c>
-    </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F55" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A56" t="s">
         <v>45</v>
       </c>
@@ -1683,8 +2039,11 @@
       <c r="E56" t="s">
         <v>105</v>
       </c>
-    </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F56" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A57" t="s">
         <v>45</v>
       </c>
@@ -1700,8 +2059,11 @@
       <c r="E57" t="s">
         <v>105</v>
       </c>
-    </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F57" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="58" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A58" t="s">
         <v>45</v>
       </c>
@@ -1717,8 +2079,11 @@
       <c r="E58" t="s">
         <v>105</v>
       </c>
-    </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F58" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="59" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A59" t="s">
         <v>45</v>
       </c>
@@ -1734,8 +2099,11 @@
       <c r="E59" t="s">
         <v>101</v>
       </c>
-    </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F59" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="60" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A60" t="s">
         <v>45</v>
       </c>
@@ -1751,8 +2119,11 @@
       <c r="E60" t="s">
         <v>102</v>
       </c>
-    </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F60" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="61" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A61" t="s">
         <v>45</v>
       </c>
@@ -1768,8 +2139,11 @@
       <c r="E61" t="s">
         <v>105</v>
       </c>
-    </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F61" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="62" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A62" t="s">
         <v>45</v>
       </c>
@@ -1785,8 +2159,11 @@
       <c r="E62" t="s">
         <v>105</v>
       </c>
-    </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F62" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="63" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A63" t="s">
         <v>45</v>
       </c>
@@ -1802,8 +2179,11 @@
       <c r="E63" t="s">
         <v>100</v>
       </c>
-    </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F63" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="64" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A64" t="s">
         <v>45</v>
       </c>
@@ -1819,8 +2199,11 @@
       <c r="E64" t="s">
         <v>101</v>
       </c>
-    </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F64" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="65" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A65" t="s">
         <v>45</v>
       </c>
@@ -1836,8 +2219,11 @@
       <c r="E65" t="s">
         <v>101</v>
       </c>
-    </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F65" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="66" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A66" t="s">
         <v>45</v>
       </c>
@@ -1853,8 +2239,11 @@
       <c r="E66" t="s">
         <v>105</v>
       </c>
-    </row>
-    <row r="67" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F66" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="67" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A67" t="s">
         <v>66</v>
       </c>
@@ -1870,8 +2259,11 @@
       <c r="E67" t="s">
         <v>100</v>
       </c>
-    </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F67" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="68" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A68" t="s">
         <v>66</v>
       </c>
@@ -1887,8 +2279,11 @@
       <c r="E68" t="s">
         <v>104</v>
       </c>
-    </row>
-    <row r="69" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F68" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="69" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A69" t="s">
         <v>66</v>
       </c>
@@ -1904,8 +2299,11 @@
       <c r="E69" t="s">
         <v>105</v>
       </c>
-    </row>
-    <row r="70" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F69" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="70" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A70" t="s">
         <v>66</v>
       </c>
@@ -1921,8 +2319,11 @@
       <c r="E70" t="s">
         <v>100</v>
       </c>
-    </row>
-    <row r="71" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F70" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="71" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A71" t="s">
         <v>66</v>
       </c>
@@ -1938,8 +2339,11 @@
       <c r="E71" t="s">
         <v>102</v>
       </c>
-    </row>
-    <row r="72" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F71" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="72" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A72" t="s">
         <v>66</v>
       </c>
@@ -1955,8 +2359,11 @@
       <c r="E72" t="s">
         <v>101</v>
       </c>
-    </row>
-    <row r="73" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F72" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="73" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A73" t="s">
         <v>66</v>
       </c>
@@ -1972,8 +2379,11 @@
       <c r="E73" t="s">
         <v>104</v>
       </c>
-    </row>
-    <row r="74" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F73" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="74" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A74" t="s">
         <v>66</v>
       </c>
@@ -1989,8 +2399,11 @@
       <c r="E74" t="s">
         <v>104</v>
       </c>
-    </row>
-    <row r="75" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F74" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="75" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A75" t="s">
         <v>66</v>
       </c>
@@ -2006,8 +2419,11 @@
       <c r="E75" t="s">
         <v>105</v>
       </c>
-    </row>
-    <row r="76" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F75" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="76" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A76" t="s">
         <v>66</v>
       </c>
@@ -2023,8 +2439,11 @@
       <c r="E76" t="s">
         <v>105</v>
       </c>
-    </row>
-    <row r="77" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F76" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="77" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A77" t="s">
         <v>76</v>
       </c>
@@ -2040,8 +2459,11 @@
       <c r="E77" t="s">
         <v>101</v>
       </c>
-    </row>
-    <row r="78" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F77" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="78" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A78" t="s">
         <v>76</v>
       </c>
@@ -2057,8 +2479,11 @@
       <c r="E78" t="s">
         <v>104</v>
       </c>
-    </row>
-    <row r="79" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F78" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="79" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A79" t="s">
         <v>76</v>
       </c>
@@ -2074,8 +2499,11 @@
       <c r="E79" t="s">
         <v>100</v>
       </c>
-    </row>
-    <row r="80" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F79" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="80" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A80" t="s">
         <v>76</v>
       </c>
@@ -2091,8 +2519,11 @@
       <c r="E80" t="s">
         <v>104</v>
       </c>
-    </row>
-    <row r="81" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F80" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="81" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A81" t="s">
         <v>76</v>
       </c>
@@ -2108,8 +2539,11 @@
       <c r="E81" t="s">
         <v>105</v>
       </c>
-    </row>
-    <row r="82" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F81" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="82" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A82" t="s">
         <v>76</v>
       </c>
@@ -2125,8 +2559,11 @@
       <c r="E82" t="s">
         <v>102</v>
       </c>
-    </row>
-    <row r="83" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F82" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="83" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A83" t="s">
         <v>76</v>
       </c>
@@ -2142,8 +2579,11 @@
       <c r="E83" t="s">
         <v>102</v>
       </c>
-    </row>
-    <row r="84" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F83" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="84" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A84" t="s">
         <v>76</v>
       </c>
@@ -2159,8 +2599,11 @@
       <c r="E84" t="s">
         <v>104</v>
       </c>
-    </row>
-    <row r="85" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F84" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="85" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A85" t="s">
         <v>76</v>
       </c>
@@ -2176,8 +2619,11 @@
       <c r="E85" t="s">
         <v>105</v>
       </c>
-    </row>
-    <row r="86" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F85" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="86" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A86" t="s">
         <v>76</v>
       </c>
@@ -2193,8 +2639,11 @@
       <c r="E86" t="s">
         <v>103</v>
       </c>
-    </row>
-    <row r="87" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F86" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="87" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A87" t="s">
         <v>85</v>
       </c>
@@ -2210,8 +2659,11 @@
       <c r="E87" t="s">
         <v>104</v>
       </c>
-    </row>
-    <row r="88" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F87" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="88" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A88" t="s">
         <v>85</v>
       </c>
@@ -2227,8 +2679,11 @@
       <c r="E88" t="s">
         <v>100</v>
       </c>
-    </row>
-    <row r="89" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F88" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="89" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A89" t="s">
         <v>85</v>
       </c>
@@ -2244,8 +2699,11 @@
       <c r="E89" t="s">
         <v>100</v>
       </c>
-    </row>
-    <row r="90" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F89" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="90" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A90" t="s">
         <v>85</v>
       </c>
@@ -2261,8 +2719,11 @@
       <c r="E90" t="s">
         <v>105</v>
       </c>
-    </row>
-    <row r="91" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F90" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="91" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A91" t="s">
         <v>85</v>
       </c>
@@ -2278,8 +2739,11 @@
       <c r="E91" t="s">
         <v>105</v>
       </c>
-    </row>
-    <row r="92" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F91" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="92" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A92" t="s">
         <v>85</v>
       </c>
@@ -2295,8 +2759,11 @@
       <c r="E92" t="s">
         <v>105</v>
       </c>
-    </row>
-    <row r="93" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F92" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="93" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A93" t="s">
         <v>85</v>
       </c>
@@ -2312,8 +2779,11 @@
       <c r="E93" t="s">
         <v>105</v>
       </c>
-    </row>
-    <row r="94" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F93" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="94" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A94" t="s">
         <v>85</v>
       </c>
@@ -2329,8 +2799,11 @@
       <c r="E94" t="s">
         <v>105</v>
       </c>
-    </row>
-    <row r="95" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F94" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="95" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A95" t="s">
         <v>85</v>
       </c>
@@ -2346,8 +2819,11 @@
       <c r="E95" t="s">
         <v>104</v>
       </c>
-    </row>
-    <row r="96" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F95" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="96" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A96" t="s">
         <v>85</v>
       </c>
@@ -2363,8 +2839,11 @@
       <c r="E96" t="s">
         <v>105</v>
       </c>
-    </row>
-    <row r="97" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F96" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="97" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A97" t="s">
         <v>85</v>
       </c>
@@ -2380,8 +2859,11 @@
       <c r="E97" t="s">
         <v>101</v>
       </c>
-    </row>
-    <row r="98" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F97" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="98" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A98" t="s">
         <v>85</v>
       </c>
@@ -2397,8 +2879,11 @@
       <c r="E98" t="s">
         <v>101</v>
       </c>
-    </row>
-    <row r="99" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F98" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="99" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A99" t="s">
         <v>85</v>
       </c>
@@ -2414,8 +2899,11 @@
       <c r="E99" t="s">
         <v>101</v>
       </c>
-    </row>
-    <row r="100" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F99" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="100" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A100" t="s">
         <v>85</v>
       </c>
@@ -2431,8 +2919,11 @@
       <c r="E100" t="s">
         <v>101</v>
       </c>
-    </row>
-    <row r="101" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F100" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="101" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A101" t="s">
         <v>85</v>
       </c>
@@ -2448,8 +2939,11 @@
       <c r="E101" t="s">
         <v>101</v>
       </c>
-    </row>
-    <row r="102" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F101" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="102" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A102" t="s">
         <v>85</v>
       </c>
@@ -2465,8 +2959,11 @@
       <c r="E102" t="s">
         <v>102</v>
       </c>
-    </row>
-    <row r="103" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F102" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="103" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A103" t="s">
         <v>85</v>
       </c>
@@ -2483,8 +2980,11 @@
       <c r="E103" t="s">
         <v>101</v>
       </c>
-    </row>
-    <row r="104" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F103" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="104" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A104" t="s">
         <v>85</v>
       </c>
@@ -2500,8 +3000,11 @@
       <c r="E104" t="s">
         <v>101</v>
       </c>
-    </row>
-    <row r="105" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F104" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="105" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A105" t="s">
         <v>85</v>
       </c>
@@ -2517,8 +3020,11 @@
       <c r="E105" t="s">
         <v>102</v>
       </c>
-    </row>
-    <row r="106" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F105" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="106" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A106" t="s">
         <v>85</v>
       </c>
@@ -2534,8 +3040,11 @@
       <c r="E106" t="s">
         <v>102</v>
       </c>
-    </row>
-    <row r="107" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F106" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="107" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A107" t="s">
         <v>95</v>
       </c>
@@ -2551,8 +3060,11 @@
       <c r="E107" t="s">
         <v>101</v>
       </c>
-    </row>
-    <row r="108" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F107" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="108" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A108" t="s">
         <v>95</v>
       </c>
@@ -2568,8 +3080,11 @@
       <c r="E108" t="s">
         <v>103</v>
       </c>
-    </row>
-    <row r="109" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F108" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="109" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A109" t="s">
         <v>95</v>
       </c>
@@ -2585,8 +3100,11 @@
       <c r="E109" t="s">
         <v>101</v>
       </c>
-    </row>
-    <row r="110" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F109" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="110" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A110" t="s">
         <v>95</v>
       </c>
@@ -2602,8 +3120,11 @@
       <c r="E110" t="s">
         <v>101</v>
       </c>
-    </row>
-    <row r="111" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F110" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="111" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A111" t="s">
         <v>95</v>
       </c>
@@ -2619,8 +3140,11 @@
       <c r="E111" t="s">
         <v>101</v>
       </c>
-    </row>
-    <row r="112" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F111" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="112" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A112" t="s">
         <v>95</v>
       </c>
@@ -2636,8 +3160,11 @@
       <c r="E112" t="s">
         <v>101</v>
       </c>
-    </row>
-    <row r="113" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F112" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="113" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A113" t="s">
         <v>95</v>
       </c>
@@ -2653,8 +3180,11 @@
       <c r="E113" t="s">
         <v>103</v>
       </c>
-    </row>
-    <row r="114" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F113" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="114" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A114" t="s">
         <v>95</v>
       </c>
@@ -2670,8 +3200,11 @@
       <c r="E114" t="s">
         <v>103</v>
       </c>
-    </row>
-    <row r="115" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F114" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="115" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A115" t="s">
         <v>95</v>
       </c>
@@ -2686,6 +3219,1801 @@
       </c>
       <c r="E115" t="s">
         <v>103</v>
+      </c>
+      <c r="F115" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="116" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A116" t="s">
+        <v>110</v>
+      </c>
+      <c r="B116" t="s">
+        <v>111</v>
+      </c>
+      <c r="C116">
+        <v>1</v>
+      </c>
+      <c r="D116" t="s">
+        <v>6</v>
+      </c>
+      <c r="E116" t="s">
+        <v>105</v>
+      </c>
+      <c r="F116" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="117" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A117" t="s">
+        <v>110</v>
+      </c>
+      <c r="B117" t="s">
+        <v>33</v>
+      </c>
+      <c r="C117">
+        <v>1</v>
+      </c>
+      <c r="D117" t="s">
+        <v>6</v>
+      </c>
+      <c r="E117" t="s">
+        <v>103</v>
+      </c>
+      <c r="F117" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="118" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A118" t="s">
+        <v>110</v>
+      </c>
+      <c r="B118" t="s">
+        <v>112</v>
+      </c>
+      <c r="C118">
+        <v>100</v>
+      </c>
+      <c r="D118" t="s">
+        <v>28</v>
+      </c>
+      <c r="E118" t="s">
+        <v>101</v>
+      </c>
+      <c r="F118" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="119" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A119" t="s">
+        <v>110</v>
+      </c>
+      <c r="B119" t="s">
+        <v>113</v>
+      </c>
+      <c r="C119">
+        <v>1000</v>
+      </c>
+      <c r="D119" t="s">
+        <v>50</v>
+      </c>
+      <c r="E119" t="s">
+        <v>101</v>
+      </c>
+      <c r="F119" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="120" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A120" t="s">
+        <v>110</v>
+      </c>
+      <c r="B120" t="s">
+        <v>114</v>
+      </c>
+      <c r="C120">
+        <v>1</v>
+      </c>
+      <c r="D120" t="s">
+        <v>6</v>
+      </c>
+      <c r="E120" t="s">
+        <v>105</v>
+      </c>
+      <c r="F120" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="121" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A121" t="s">
+        <v>110</v>
+      </c>
+      <c r="B121" t="s">
+        <v>24</v>
+      </c>
+      <c r="C121">
+        <v>1</v>
+      </c>
+      <c r="D121" t="s">
+        <v>6</v>
+      </c>
+      <c r="E121" t="s">
+        <v>105</v>
+      </c>
+      <c r="F121" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="122" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A122" t="s">
+        <v>110</v>
+      </c>
+      <c r="B122" t="s">
+        <v>44</v>
+      </c>
+      <c r="C122">
+        <v>3</v>
+      </c>
+      <c r="D122" t="s">
+        <v>7</v>
+      </c>
+      <c r="E122" t="s">
+        <v>102</v>
+      </c>
+      <c r="F122" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="123" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A123" t="s">
+        <v>116</v>
+      </c>
+      <c r="B123" t="s">
+        <v>117</v>
+      </c>
+      <c r="C123">
+        <v>6</v>
+      </c>
+      <c r="D123" t="s">
+        <v>7</v>
+      </c>
+      <c r="E123" t="s">
+        <v>101</v>
+      </c>
+      <c r="F123" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="124" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A124" t="s">
+        <v>116</v>
+      </c>
+      <c r="B124" t="s">
+        <v>57</v>
+      </c>
+      <c r="C124">
+        <v>1</v>
+      </c>
+      <c r="D124" t="s">
+        <v>6</v>
+      </c>
+      <c r="E124" t="s">
+        <v>105</v>
+      </c>
+      <c r="F124" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="125" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A125" t="s">
+        <v>116</v>
+      </c>
+      <c r="B125" t="s">
+        <v>118</v>
+      </c>
+      <c r="C125">
+        <v>1</v>
+      </c>
+      <c r="D125" t="s">
+        <v>6</v>
+      </c>
+      <c r="E125" t="s">
+        <v>105</v>
+      </c>
+      <c r="F125" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="126" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A126" t="s">
+        <v>116</v>
+      </c>
+      <c r="B126" t="s">
+        <v>51</v>
+      </c>
+      <c r="C126">
+        <v>4</v>
+      </c>
+      <c r="D126" t="s">
+        <v>52</v>
+      </c>
+      <c r="E126" t="s">
+        <v>105</v>
+      </c>
+      <c r="F126" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="127" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A127" t="s">
+        <v>116</v>
+      </c>
+      <c r="B127" t="s">
+        <v>119</v>
+      </c>
+      <c r="C127">
+        <v>2</v>
+      </c>
+      <c r="D127" t="s">
+        <v>7</v>
+      </c>
+      <c r="E127" t="s">
+        <v>159</v>
+      </c>
+      <c r="F127" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="128" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A128" t="s">
+        <v>116</v>
+      </c>
+      <c r="B128" t="s">
+        <v>120</v>
+      </c>
+      <c r="C128">
+        <v>1</v>
+      </c>
+      <c r="D128" t="s">
+        <v>7</v>
+      </c>
+      <c r="E128" t="s">
+        <v>159</v>
+      </c>
+      <c r="F128" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="129" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A129" t="s">
+        <v>116</v>
+      </c>
+      <c r="B129" t="s">
+        <v>81</v>
+      </c>
+      <c r="C129">
+        <v>0.25</v>
+      </c>
+      <c r="D129" t="s">
+        <v>7</v>
+      </c>
+      <c r="E129" t="s">
+        <v>159</v>
+      </c>
+      <c r="F129" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="130" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A130" t="s">
+        <v>116</v>
+      </c>
+      <c r="B130" t="s">
+        <v>111</v>
+      </c>
+      <c r="C130">
+        <v>1</v>
+      </c>
+      <c r="D130" t="s">
+        <v>121</v>
+      </c>
+      <c r="E130" t="s">
+        <v>105</v>
+      </c>
+      <c r="F130" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="131" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A131" t="s">
+        <v>116</v>
+      </c>
+      <c r="B131" t="s">
+        <v>33</v>
+      </c>
+      <c r="C131">
+        <v>6</v>
+      </c>
+      <c r="D131" t="s">
+        <v>6</v>
+      </c>
+      <c r="E131" t="s">
+        <v>103</v>
+      </c>
+      <c r="F131" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="132" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A132" t="s">
+        <v>116</v>
+      </c>
+      <c r="B132" t="s">
+        <v>114</v>
+      </c>
+      <c r="C132">
+        <v>1</v>
+      </c>
+      <c r="D132" t="s">
+        <v>6</v>
+      </c>
+      <c r="E132" t="s">
+        <v>105</v>
+      </c>
+      <c r="F132" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="133" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A133" t="s">
+        <v>116</v>
+      </c>
+      <c r="B133" t="s">
+        <v>122</v>
+      </c>
+      <c r="C133">
+        <v>1</v>
+      </c>
+      <c r="D133" t="s">
+        <v>6</v>
+      </c>
+      <c r="E133" t="s">
+        <v>105</v>
+      </c>
+      <c r="F133" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="134" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A134" t="s">
+        <v>124</v>
+      </c>
+      <c r="B134" t="s">
+        <v>125</v>
+      </c>
+      <c r="C134">
+        <v>1</v>
+      </c>
+      <c r="D134" t="s">
+        <v>6</v>
+      </c>
+      <c r="E134" t="s">
+        <v>105</v>
+      </c>
+      <c r="F134" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="135" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A135" t="s">
+        <v>124</v>
+      </c>
+      <c r="B135" t="s">
+        <v>126</v>
+      </c>
+      <c r="C135">
+        <v>1</v>
+      </c>
+      <c r="D135" t="s">
+        <v>6</v>
+      </c>
+      <c r="E135" t="s">
+        <v>100</v>
+      </c>
+      <c r="F135" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="136" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A136" t="s">
+        <v>124</v>
+      </c>
+      <c r="B136" t="s">
+        <v>127</v>
+      </c>
+      <c r="C136">
+        <v>0.5</v>
+      </c>
+      <c r="D136" t="s">
+        <v>128</v>
+      </c>
+      <c r="E136" t="s">
+        <v>105</v>
+      </c>
+      <c r="F136" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="137" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A137" t="s">
+        <v>124</v>
+      </c>
+      <c r="B137" t="s">
+        <v>117</v>
+      </c>
+      <c r="C137">
+        <v>3</v>
+      </c>
+      <c r="D137" t="s">
+        <v>7</v>
+      </c>
+      <c r="E137" s="3" t="s">
+        <v>102</v>
+      </c>
+      <c r="F137" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="138" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A138" t="s">
+        <v>124</v>
+      </c>
+      <c r="B138" t="s">
+        <v>129</v>
+      </c>
+      <c r="C138">
+        <v>1</v>
+      </c>
+      <c r="D138" t="s">
+        <v>6</v>
+      </c>
+      <c r="E138" t="s">
+        <v>105</v>
+      </c>
+      <c r="F138" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="139" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A139" t="s">
+        <v>124</v>
+      </c>
+      <c r="B139" t="s">
+        <v>130</v>
+      </c>
+      <c r="C139">
+        <v>3</v>
+      </c>
+      <c r="D139" t="s">
+        <v>7</v>
+      </c>
+      <c r="E139" t="s">
+        <v>101</v>
+      </c>
+      <c r="F139" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="140" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A140" t="s">
+        <v>131</v>
+      </c>
+      <c r="B140" t="s">
+        <v>33</v>
+      </c>
+      <c r="C140">
+        <v>4</v>
+      </c>
+      <c r="D140" t="s">
+        <v>6</v>
+      </c>
+      <c r="E140" t="s">
+        <v>103</v>
+      </c>
+      <c r="F140" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="141" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A141" t="s">
+        <v>131</v>
+      </c>
+      <c r="B141" t="s">
+        <v>24</v>
+      </c>
+      <c r="C141">
+        <v>2</v>
+      </c>
+      <c r="D141" t="s">
+        <v>6</v>
+      </c>
+      <c r="E141" t="s">
+        <v>105</v>
+      </c>
+      <c r="F141" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="142" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A142" t="s">
+        <v>131</v>
+      </c>
+      <c r="B142" t="s">
+        <v>35</v>
+      </c>
+      <c r="C142">
+        <v>1</v>
+      </c>
+      <c r="D142" t="s">
+        <v>7</v>
+      </c>
+      <c r="E142" t="s">
+        <v>101</v>
+      </c>
+      <c r="F142" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="143" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A143" t="s">
+        <v>131</v>
+      </c>
+      <c r="B143" t="s">
+        <v>93</v>
+      </c>
+      <c r="C143">
+        <v>0.5</v>
+      </c>
+      <c r="D143" t="s">
+        <v>7</v>
+      </c>
+      <c r="E143" t="s">
+        <v>159</v>
+      </c>
+      <c r="F143" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="144" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A144" t="s">
+        <v>131</v>
+      </c>
+      <c r="B144" t="s">
+        <v>11</v>
+      </c>
+      <c r="C144">
+        <v>1</v>
+      </c>
+      <c r="D144" t="s">
+        <v>7</v>
+      </c>
+      <c r="E144" t="s">
+        <v>101</v>
+      </c>
+      <c r="F144" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="145" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A145" t="s">
+        <v>131</v>
+      </c>
+      <c r="B145" t="s">
+        <v>72</v>
+      </c>
+      <c r="C145">
+        <v>1</v>
+      </c>
+      <c r="D145" t="s">
+        <v>7</v>
+      </c>
+      <c r="E145" t="s">
+        <v>159</v>
+      </c>
+      <c r="F145" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="146" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A146" t="s">
+        <v>133</v>
+      </c>
+      <c r="B146" t="s">
+        <v>134</v>
+      </c>
+      <c r="C146">
+        <v>2</v>
+      </c>
+      <c r="D146" t="s">
+        <v>6</v>
+      </c>
+      <c r="E146" t="s">
+        <v>159</v>
+      </c>
+      <c r="F146" t="s">
+        <v>108</v>
+      </c>
+      <c r="G146" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="147" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A147" t="s">
+        <v>133</v>
+      </c>
+      <c r="B147" t="s">
+        <v>61</v>
+      </c>
+      <c r="C147">
+        <v>2</v>
+      </c>
+      <c r="D147" t="s">
+        <v>6</v>
+      </c>
+      <c r="E147" t="s">
+        <v>159</v>
+      </c>
+      <c r="F147" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="148" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A148" t="s">
+        <v>133</v>
+      </c>
+      <c r="B148" t="s">
+        <v>135</v>
+      </c>
+      <c r="C148">
+        <v>2</v>
+      </c>
+      <c r="D148" t="s">
+        <v>6</v>
+      </c>
+      <c r="E148" t="s">
+        <v>159</v>
+      </c>
+      <c r="F148" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="149" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A149" t="s">
+        <v>133</v>
+      </c>
+      <c r="B149" t="s">
+        <v>136</v>
+      </c>
+      <c r="C149">
+        <v>2</v>
+      </c>
+      <c r="D149" t="s">
+        <v>6</v>
+      </c>
+      <c r="E149" t="s">
+        <v>159</v>
+      </c>
+      <c r="F149" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="150" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A150" t="s">
+        <v>133</v>
+      </c>
+      <c r="B150" t="s">
+        <v>137</v>
+      </c>
+      <c r="C150">
+        <v>3</v>
+      </c>
+      <c r="D150" t="s">
+        <v>7</v>
+      </c>
+      <c r="E150" t="s">
+        <v>159</v>
+      </c>
+      <c r="F150" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="151" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A151" t="s">
+        <v>133</v>
+      </c>
+      <c r="B151" t="s">
+        <v>138</v>
+      </c>
+      <c r="C151">
+        <v>1</v>
+      </c>
+      <c r="D151" t="s">
+        <v>7</v>
+      </c>
+      <c r="E151" t="s">
+        <v>159</v>
+      </c>
+      <c r="F151" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="152" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A152" t="s">
+        <v>133</v>
+      </c>
+      <c r="B152" t="s">
+        <v>139</v>
+      </c>
+      <c r="C152">
+        <v>3</v>
+      </c>
+      <c r="D152" t="s">
+        <v>7</v>
+      </c>
+      <c r="E152" t="s">
+        <v>159</v>
+      </c>
+      <c r="F152" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="153" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A153" t="s">
+        <v>133</v>
+      </c>
+      <c r="B153" t="s">
+        <v>140</v>
+      </c>
+      <c r="C153">
+        <v>650</v>
+      </c>
+      <c r="D153" t="s">
+        <v>28</v>
+      </c>
+      <c r="E153" t="s">
+        <v>100</v>
+      </c>
+      <c r="F153" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="154" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A154" t="s">
+        <v>133</v>
+      </c>
+      <c r="B154" t="s">
+        <v>11</v>
+      </c>
+      <c r="C154">
+        <v>18</v>
+      </c>
+      <c r="D154" t="s">
+        <v>7</v>
+      </c>
+      <c r="E154" t="s">
+        <v>101</v>
+      </c>
+      <c r="F154" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="155" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A155" t="s">
+        <v>133</v>
+      </c>
+      <c r="B155" t="s">
+        <v>51</v>
+      </c>
+      <c r="C155">
+        <v>18</v>
+      </c>
+      <c r="D155" t="s">
+        <v>52</v>
+      </c>
+      <c r="E155" t="s">
+        <v>105</v>
+      </c>
+      <c r="F155" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="156" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A156" t="s">
+        <v>133</v>
+      </c>
+      <c r="B156" t="s">
+        <v>42</v>
+      </c>
+      <c r="C156">
+        <v>2</v>
+      </c>
+      <c r="D156" t="s">
+        <v>41</v>
+      </c>
+      <c r="E156" t="s">
+        <v>105</v>
+      </c>
+      <c r="F156" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="157" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A157" t="s">
+        <v>133</v>
+      </c>
+      <c r="B157" t="s">
+        <v>57</v>
+      </c>
+      <c r="C157">
+        <v>0.5</v>
+      </c>
+      <c r="D157" t="s">
+        <v>6</v>
+      </c>
+      <c r="E157" t="s">
+        <v>105</v>
+      </c>
+      <c r="F157" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="158" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A158" t="s">
+        <v>133</v>
+      </c>
+      <c r="B158" t="s">
+        <v>24</v>
+      </c>
+      <c r="C158">
+        <v>5</v>
+      </c>
+      <c r="D158" t="s">
+        <v>6</v>
+      </c>
+      <c r="E158" t="s">
+        <v>105</v>
+      </c>
+      <c r="F158" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="159" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A159" t="s">
+        <v>133</v>
+      </c>
+      <c r="B159" t="s">
+        <v>15</v>
+      </c>
+      <c r="C159">
+        <v>6</v>
+      </c>
+      <c r="D159" t="s">
+        <v>7</v>
+      </c>
+      <c r="E159" t="s">
+        <v>101</v>
+      </c>
+      <c r="F159" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="160" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A160" t="s">
+        <v>133</v>
+      </c>
+      <c r="B160" t="s">
+        <v>16</v>
+      </c>
+      <c r="C160">
+        <v>0.5</v>
+      </c>
+      <c r="D160" t="s">
+        <v>32</v>
+      </c>
+      <c r="E160" t="s">
+        <v>102</v>
+      </c>
+      <c r="F160" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="161" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A161" t="s">
+        <v>133</v>
+      </c>
+      <c r="B161" t="s">
+        <v>141</v>
+      </c>
+      <c r="C161">
+        <v>0.5</v>
+      </c>
+      <c r="D161" t="s">
+        <v>32</v>
+      </c>
+      <c r="E161" t="s">
+        <v>102</v>
+      </c>
+      <c r="F161" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="162" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A162" t="s">
+        <v>133</v>
+      </c>
+      <c r="B162" t="s">
+        <v>142</v>
+      </c>
+      <c r="C162">
+        <v>3</v>
+      </c>
+      <c r="D162" t="s">
+        <v>7</v>
+      </c>
+      <c r="E162" t="s">
+        <v>102</v>
+      </c>
+      <c r="F162" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="163" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A163" t="s">
+        <v>133</v>
+      </c>
+      <c r="B163" t="s">
+        <v>35</v>
+      </c>
+      <c r="C163">
+        <v>0.5</v>
+      </c>
+      <c r="D163" t="s">
+        <v>7</v>
+      </c>
+      <c r="E163" t="s">
+        <v>101</v>
+      </c>
+      <c r="F163" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="164" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A164" t="s">
+        <v>133</v>
+      </c>
+      <c r="B164" t="s">
+        <v>111</v>
+      </c>
+      <c r="C164">
+        <v>2</v>
+      </c>
+      <c r="D164" t="s">
+        <v>6</v>
+      </c>
+      <c r="E164" t="s">
+        <v>105</v>
+      </c>
+      <c r="F164" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="165" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A165" t="s">
+        <v>133</v>
+      </c>
+      <c r="B165" t="s">
+        <v>143</v>
+      </c>
+      <c r="C165">
+        <v>2</v>
+      </c>
+      <c r="D165" t="s">
+        <v>7</v>
+      </c>
+      <c r="E165" t="s">
+        <v>101</v>
+      </c>
+      <c r="F165" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="166" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A166" t="s">
+        <v>133</v>
+      </c>
+      <c r="B166" t="s">
+        <v>89</v>
+      </c>
+      <c r="C166">
+        <v>1</v>
+      </c>
+      <c r="D166" t="s">
+        <v>6</v>
+      </c>
+      <c r="E166" t="s">
+        <v>105</v>
+      </c>
+      <c r="F166" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="167" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A167" t="s">
+        <v>133</v>
+      </c>
+      <c r="B167" t="s">
+        <v>144</v>
+      </c>
+      <c r="C167">
+        <v>1</v>
+      </c>
+      <c r="D167" t="s">
+        <v>145</v>
+      </c>
+      <c r="E167" t="s">
+        <v>101</v>
+      </c>
+      <c r="F167" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="168" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A168" t="s">
+        <v>133</v>
+      </c>
+      <c r="B168" t="s">
+        <v>24</v>
+      </c>
+      <c r="C168">
+        <v>1</v>
+      </c>
+      <c r="D168" t="s">
+        <v>6</v>
+      </c>
+      <c r="E168" t="s">
+        <v>105</v>
+      </c>
+      <c r="F168" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="169" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A169" t="s">
+        <v>133</v>
+      </c>
+      <c r="B169" t="s">
+        <v>114</v>
+      </c>
+      <c r="C169">
+        <v>1</v>
+      </c>
+      <c r="D169" t="s">
+        <v>6</v>
+      </c>
+      <c r="E169" t="s">
+        <v>105</v>
+      </c>
+      <c r="F169" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="170" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A170" t="s">
+        <v>147</v>
+      </c>
+      <c r="B170" t="s">
+        <v>57</v>
+      </c>
+      <c r="C170">
+        <v>2</v>
+      </c>
+      <c r="D170" t="s">
+        <v>6</v>
+      </c>
+      <c r="E170" t="s">
+        <v>105</v>
+      </c>
+      <c r="F170" t="s">
+        <v>108</v>
+      </c>
+      <c r="G170" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="171" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A171" t="s">
+        <v>147</v>
+      </c>
+      <c r="B171" t="s">
+        <v>42</v>
+      </c>
+      <c r="C171">
+        <v>150</v>
+      </c>
+      <c r="D171" t="s">
+        <v>28</v>
+      </c>
+      <c r="E171" t="s">
+        <v>105</v>
+      </c>
+      <c r="F171" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="172" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A172" t="s">
+        <v>147</v>
+      </c>
+      <c r="B172" t="s">
+        <v>135</v>
+      </c>
+      <c r="C172">
+        <v>10</v>
+      </c>
+      <c r="D172" t="s">
+        <v>6</v>
+      </c>
+      <c r="E172" t="s">
+        <v>159</v>
+      </c>
+      <c r="F172" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="173" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A173" t="s">
+        <v>147</v>
+      </c>
+      <c r="B173" t="s">
+        <v>39</v>
+      </c>
+      <c r="C173">
+        <v>3</v>
+      </c>
+      <c r="D173" t="s">
+        <v>7</v>
+      </c>
+      <c r="E173" t="s">
+        <v>159</v>
+      </c>
+      <c r="F173" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="174" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A174" t="s">
+        <v>147</v>
+      </c>
+      <c r="B174" t="s">
+        <v>134</v>
+      </c>
+      <c r="C174">
+        <v>3</v>
+      </c>
+      <c r="D174" t="s">
+        <v>6</v>
+      </c>
+      <c r="E174" t="s">
+        <v>159</v>
+      </c>
+      <c r="F174" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="175" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A175" t="s">
+        <v>147</v>
+      </c>
+      <c r="B175" t="s">
+        <v>52</v>
+      </c>
+      <c r="C175">
+        <v>3</v>
+      </c>
+      <c r="D175" t="s">
+        <v>6</v>
+      </c>
+      <c r="E175" t="s">
+        <v>159</v>
+      </c>
+      <c r="F175" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="176" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A176" t="s">
+        <v>147</v>
+      </c>
+      <c r="B176" t="s">
+        <v>148</v>
+      </c>
+      <c r="C176">
+        <v>4.5</v>
+      </c>
+      <c r="D176" t="s">
+        <v>7</v>
+      </c>
+      <c r="E176" t="s">
+        <v>159</v>
+      </c>
+      <c r="F176" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="177" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A177" t="s">
+        <v>147</v>
+      </c>
+      <c r="B177" t="s">
+        <v>149</v>
+      </c>
+      <c r="C177">
+        <v>1500</v>
+      </c>
+      <c r="D177" t="s">
+        <v>28</v>
+      </c>
+      <c r="E177" t="s">
+        <v>100</v>
+      </c>
+      <c r="F177" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="178" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A178" t="s">
+        <v>147</v>
+      </c>
+      <c r="B178" t="s">
+        <v>150</v>
+      </c>
+      <c r="C178">
+        <v>1000</v>
+      </c>
+      <c r="D178" t="s">
+        <v>28</v>
+      </c>
+      <c r="E178" t="s">
+        <v>100</v>
+      </c>
+      <c r="F178" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="179" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A179" t="s">
+        <v>147</v>
+      </c>
+      <c r="B179" t="s">
+        <v>151</v>
+      </c>
+      <c r="C179">
+        <v>1000</v>
+      </c>
+      <c r="D179" t="s">
+        <v>28</v>
+      </c>
+      <c r="E179" t="s">
+        <v>100</v>
+      </c>
+      <c r="F179" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="180" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A180" t="s">
+        <v>147</v>
+      </c>
+      <c r="B180" t="s">
+        <v>15</v>
+      </c>
+      <c r="C180">
+        <v>6</v>
+      </c>
+      <c r="D180" t="s">
+        <v>7</v>
+      </c>
+      <c r="E180" t="s">
+        <v>101</v>
+      </c>
+      <c r="F180" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="181" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A181" t="s">
+        <v>147</v>
+      </c>
+      <c r="B181" t="s">
+        <v>152</v>
+      </c>
+      <c r="C181">
+        <v>40</v>
+      </c>
+      <c r="D181" t="s">
+        <v>50</v>
+      </c>
+      <c r="E181" t="s">
+        <v>101</v>
+      </c>
+      <c r="F181" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="182" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A182" t="s">
+        <v>147</v>
+      </c>
+      <c r="B182" t="s">
+        <v>153</v>
+      </c>
+      <c r="C182">
+        <v>60</v>
+      </c>
+      <c r="D182" t="s">
+        <v>28</v>
+      </c>
+      <c r="E182" t="s">
+        <v>100</v>
+      </c>
+      <c r="F182" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="183" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A183" t="s">
+        <v>147</v>
+      </c>
+      <c r="B183" t="s">
+        <v>154</v>
+      </c>
+      <c r="C183">
+        <v>1</v>
+      </c>
+      <c r="D183" t="s">
+        <v>6</v>
+      </c>
+      <c r="E183" t="s">
+        <v>105</v>
+      </c>
+      <c r="F183" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="184" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A184" t="s">
+        <v>147</v>
+      </c>
+      <c r="B184" t="s">
+        <v>155</v>
+      </c>
+      <c r="C184">
+        <v>5</v>
+      </c>
+      <c r="D184" t="s">
+        <v>6</v>
+      </c>
+      <c r="E184" t="s">
+        <v>105</v>
+      </c>
+      <c r="F184" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="185" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A185" t="s">
+        <v>147</v>
+      </c>
+      <c r="B185" t="s">
+        <v>114</v>
+      </c>
+      <c r="C185">
+        <v>1</v>
+      </c>
+      <c r="D185" t="s">
+        <v>6</v>
+      </c>
+      <c r="E185" t="s">
+        <v>105</v>
+      </c>
+      <c r="F185" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="186" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A186" t="s">
+        <v>147</v>
+      </c>
+      <c r="B186" t="s">
+        <v>156</v>
+      </c>
+      <c r="C186">
+        <v>1</v>
+      </c>
+      <c r="D186" t="s">
+        <v>6</v>
+      </c>
+      <c r="E186" t="s">
+        <v>105</v>
+      </c>
+      <c r="F186" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="187" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A187" t="s">
+        <v>147</v>
+      </c>
+      <c r="B187" t="s">
+        <v>157</v>
+      </c>
+      <c r="C187">
+        <v>3</v>
+      </c>
+      <c r="D187" t="s">
+        <v>7</v>
+      </c>
+      <c r="E187" t="s">
+        <v>102</v>
+      </c>
+      <c r="F187" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="188" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A188" t="s">
+        <v>147</v>
+      </c>
+      <c r="B188" t="s">
+        <v>158</v>
+      </c>
+      <c r="C188">
+        <v>3</v>
+      </c>
+      <c r="D188" t="s">
+        <v>7</v>
+      </c>
+      <c r="E188" t="s">
+        <v>102</v>
+      </c>
+      <c r="F188" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="189" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A189" t="s">
+        <v>165</v>
+      </c>
+      <c r="B189" t="s">
+        <v>161</v>
+      </c>
+      <c r="C189">
+        <v>100</v>
+      </c>
+      <c r="D189" t="s">
+        <v>28</v>
+      </c>
+      <c r="E189" t="s">
+        <v>100</v>
+      </c>
+      <c r="F189" t="s">
+        <v>108</v>
+      </c>
+      <c r="G189" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="190" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A190" t="s">
+        <v>165</v>
+      </c>
+      <c r="B190" t="s">
+        <v>162</v>
+      </c>
+      <c r="C190">
+        <v>50</v>
+      </c>
+      <c r="D190" t="s">
+        <v>28</v>
+      </c>
+      <c r="E190" t="s">
+        <v>103</v>
+      </c>
+      <c r="F190" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="191" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A191" t="s">
+        <v>165</v>
+      </c>
+      <c r="B191" t="s">
+        <v>163</v>
+      </c>
+      <c r="C191">
+        <v>50</v>
+      </c>
+      <c r="D191" t="s">
+        <v>28</v>
+      </c>
+      <c r="E191" t="s">
+        <v>103</v>
+      </c>
+      <c r="F191" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="192" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A192" t="s">
+        <v>165</v>
+      </c>
+      <c r="B192" t="s">
+        <v>33</v>
+      </c>
+      <c r="C192">
+        <v>3</v>
+      </c>
+      <c r="D192" t="s">
+        <v>6</v>
+      </c>
+      <c r="E192" t="s">
+        <v>103</v>
+      </c>
+      <c r="F192" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="193" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A193" t="s">
+        <v>165</v>
+      </c>
+      <c r="B193" t="s">
+        <v>164</v>
+      </c>
+      <c r="C193">
+        <v>350</v>
+      </c>
+      <c r="D193" t="s">
+        <v>28</v>
+      </c>
+      <c r="E193" t="s">
+        <v>101</v>
+      </c>
+      <c r="F193" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="194" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A194" t="s">
+        <v>165</v>
+      </c>
+      <c r="B194" t="s">
+        <v>51</v>
+      </c>
+      <c r="C194">
+        <v>2</v>
+      </c>
+      <c r="D194" t="s">
+        <v>6</v>
+      </c>
+      <c r="E194" t="s">
+        <v>105</v>
+      </c>
+      <c r="F194" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="195" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A195" t="s">
+        <v>165</v>
+      </c>
+      <c r="B195" t="s">
+        <v>12</v>
+      </c>
+      <c r="C195">
+        <v>50</v>
+      </c>
+      <c r="D195" t="s">
+        <v>28</v>
+      </c>
+      <c r="E195" t="s">
+        <v>103</v>
+      </c>
+      <c r="F195" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="196" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A196" t="s">
+        <v>169</v>
+      </c>
+      <c r="B196" t="s">
+        <v>33</v>
+      </c>
+      <c r="C196">
+        <v>3</v>
+      </c>
+      <c r="D196" t="s">
+        <v>6</v>
+      </c>
+      <c r="E196" t="s">
+        <v>103</v>
+      </c>
+      <c r="F196" t="s">
+        <v>108</v>
+      </c>
+      <c r="G196" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="197" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A197" t="s">
+        <v>169</v>
+      </c>
+      <c r="B197" t="s">
+        <v>92</v>
+      </c>
+      <c r="C197">
+        <v>9</v>
+      </c>
+      <c r="D197" t="s">
+        <v>7</v>
+      </c>
+      <c r="E197" t="s">
+        <v>101</v>
+      </c>
+      <c r="F197" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="198" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A198" t="s">
+        <v>169</v>
+      </c>
+      <c r="B198" t="s">
+        <v>166</v>
+      </c>
+      <c r="C198">
+        <v>2</v>
+      </c>
+      <c r="D198" t="s">
+        <v>41</v>
+      </c>
+      <c r="E198" t="s">
+        <v>105</v>
+      </c>
+      <c r="F198" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="199" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A199" t="s">
+        <v>169</v>
+      </c>
+      <c r="B199" t="s">
+        <v>167</v>
+      </c>
+      <c r="C199">
+        <v>2</v>
+      </c>
+      <c r="D199" t="s">
+        <v>41</v>
+      </c>
+      <c r="E199" t="s">
+        <v>105</v>
+      </c>
+      <c r="F199" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="200" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A200" t="s">
+        <v>169</v>
+      </c>
+      <c r="B200" t="s">
+        <v>75</v>
+      </c>
+      <c r="C200">
+        <v>2</v>
+      </c>
+      <c r="D200" t="s">
+        <v>41</v>
+      </c>
+      <c r="E200" t="s">
+        <v>105</v>
+      </c>
+      <c r="F200" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="201" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A201" t="s">
+        <v>169</v>
+      </c>
+      <c r="B201" t="s">
+        <v>24</v>
+      </c>
+      <c r="C201">
+        <v>2</v>
+      </c>
+      <c r="D201" t="s">
+        <v>6</v>
+      </c>
+      <c r="E201" t="s">
+        <v>105</v>
+      </c>
+      <c r="F201" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="202" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A202" t="s">
+        <v>169</v>
+      </c>
+      <c r="B202" t="s">
+        <v>93</v>
+      </c>
+      <c r="C202">
+        <v>1</v>
+      </c>
+      <c r="D202" t="s">
+        <v>7</v>
+      </c>
+      <c r="E202" t="s">
+        <v>101</v>
+      </c>
+      <c r="F202" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="203" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A203" t="s">
+        <v>169</v>
+      </c>
+      <c r="B203" t="s">
+        <v>72</v>
+      </c>
+      <c r="C203">
+        <v>1</v>
+      </c>
+      <c r="D203" t="s">
+        <v>7</v>
+      </c>
+      <c r="E203" t="s">
+        <v>101</v>
+      </c>
+      <c r="F203" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="204" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A204" t="s">
+        <v>169</v>
+      </c>
+      <c r="B204" t="s">
+        <v>44</v>
+      </c>
+      <c r="C204">
+        <v>1</v>
+      </c>
+      <c r="D204" t="s">
+        <v>7</v>
+      </c>
+      <c r="E204" t="s">
+        <v>102</v>
+      </c>
+      <c r="F204" t="s">
+        <v>108</v>
       </c>
     </row>
   </sheetData>

</xml_diff>